<commit_message>
Assertions, Read excel, retryanalyzer, parallel execution
</commit_message>
<xml_diff>
--- a/data/CreateLead.xlsx
+++ b/data/CreateLead.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>cname</t>
   </si>
@@ -38,49 +38,13 @@
     <t>lname</t>
   </si>
   <si>
-    <t>WPS1</t>
+    <t>tcs</t>
   </si>
   <si>
-    <t>Doc1</t>
+    <t>tata</t>
   </si>
   <si>
-    <t>Pdf1</t>
-  </si>
-  <si>
-    <t>WPS2</t>
-  </si>
-  <si>
-    <t>Doc2</t>
-  </si>
-  <si>
-    <t>Pdf2</t>
-  </si>
-  <si>
-    <t>WPS3</t>
-  </si>
-  <si>
-    <t>Doc3</t>
-  </si>
-  <si>
-    <t>Pdf3</t>
-  </si>
-  <si>
-    <t>WPS4</t>
-  </si>
-  <si>
-    <t>Doc4</t>
-  </si>
-  <si>
-    <t>Pdf4</t>
-  </si>
-  <si>
-    <t>WPS5</t>
-  </si>
-  <si>
-    <t>Doc5</t>
-  </si>
-  <si>
-    <t>Pdf5</t>
+    <t>services</t>
   </si>
 </sst>
 </file>
@@ -1251,13 +1215,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -1281,50 +1245,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>